<commit_message>
udpate results visualization files
</commit_message>
<xml_diff>
--- a/scripts/GLUCOSE_configuration.xlsx
+++ b/scripts/GLUCOSE_configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agnese/Documents/KTH-Work/KTH-dESA:GLUCOSE_GitHub/GLUCOSE/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B87876C-E47E-1349-A1D4-22A6E366E428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFC425A-4F1C-374E-8E59-8704C82344E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{11C35186-7494-9D4D-BDF1-6461A1F99797}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{11C35186-7494-9D4D-BDF1-6461A1F99797}"/>
   </bookViews>
   <sheets>
     <sheet name="Technologies" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="200">
   <si>
     <t>ALU</t>
   </si>
@@ -631,6 +631,12 @@
   </si>
   <si>
     <t>EnergyFuel</t>
+  </si>
+  <si>
+    <t>gas</t>
+  </si>
+  <si>
+    <t>gas_CCS</t>
   </si>
 </sst>
 </file>
@@ -1024,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE92352E-6EA3-6D4D-A01C-D80F345E92DF}">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45:D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1795,7 +1801,7 @@
         <v>193</v>
       </c>
       <c r="D39" t="s">
-        <v>147</v>
+        <v>198</v>
       </c>
       <c r="E39" t="s">
         <v>189</v>
@@ -1815,7 +1821,7 @@
         <v>193</v>
       </c>
       <c r="D40" t="s">
-        <v>147</v>
+        <v>198</v>
       </c>
       <c r="E40" t="s">
         <v>145</v>
@@ -1835,7 +1841,7 @@
         <v>193</v>
       </c>
       <c r="D41" t="s">
-        <v>147</v>
+        <v>198</v>
       </c>
       <c r="E41" t="s">
         <v>145</v>
@@ -1855,7 +1861,7 @@
         <v>193</v>
       </c>
       <c r="D42" t="s">
-        <v>147</v>
+        <v>198</v>
       </c>
       <c r="E42" t="s">
         <v>144</v>
@@ -1875,7 +1881,7 @@
         <v>193</v>
       </c>
       <c r="D43" t="s">
-        <v>147</v>
+        <v>198</v>
       </c>
       <c r="E43" t="s">
         <v>182</v>
@@ -1895,7 +1901,7 @@
         <v>193</v>
       </c>
       <c r="D44" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="E44" t="s">
         <v>144</v>
@@ -1915,7 +1921,7 @@
         <v>193</v>
       </c>
       <c r="D45" t="s">
-        <v>147</v>
+        <v>198</v>
       </c>
       <c r="E45" t="s">
         <v>144</v>
@@ -1935,7 +1941,7 @@
         <v>193</v>
       </c>
       <c r="D46" t="s">
-        <v>147</v>
+        <v>198</v>
       </c>
       <c r="E46" t="s">
         <v>182</v>
@@ -1955,7 +1961,7 @@
         <v>193</v>
       </c>
       <c r="D47" t="s">
-        <v>147</v>
+        <v>198</v>
       </c>
       <c r="E47" t="s">
         <v>154</v>
@@ -1975,7 +1981,7 @@
         <v>193</v>
       </c>
       <c r="D48" t="s">
-        <v>147</v>
+        <v>198</v>
       </c>
       <c r="E48" t="s">
         <v>149</v>
@@ -2712,8 +2718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFBDB2AA-BBD1-964A-AE78-B4CF63DCE296}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2871,7 +2877,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>147</v>
+        <v>198</v>
       </c>
       <c r="C12" t="s">
         <v>152</v>

</xml_diff>

<commit_message>
added fuel naming convention on README.md and GLUCOSE_configuration.xlsx files
</commit_message>
<xml_diff>
--- a/scripts/GLUCOSE_configuration.xlsx
+++ b/scripts/GLUCOSE_configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agnese/Documents/KTH-Work/GitHub_repositories/KTH-dESA/GLUCOSE/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94FDFA6-7634-F24A-8A9E-BDE8604FB3D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCCD71B-84B8-224F-8914-A0ADAAC9AFE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{11C35186-7494-9D4D-BDF1-6461A1F99797}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2163" uniqueCount="434">
   <si>
     <t>ALU</t>
   </si>
@@ -1314,6 +1314,36 @@
   </si>
   <si>
     <t>Full name</t>
+  </si>
+  <si>
+    <t>Resource Level</t>
+  </si>
+  <si>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>MFOO_P_LAPS</t>
+  </si>
+  <si>
+    <t>VFOO_P_LAC</t>
+  </si>
+  <si>
+    <t>LAPS</t>
+  </si>
+  <si>
+    <t>LAC</t>
+  </si>
+  <si>
+    <t>Pasture land</t>
+  </si>
+  <si>
+    <t>Cropland</t>
+  </si>
+  <si>
+    <t>Agriculture land, Pasture</t>
+  </si>
+  <si>
+    <t>Agriculture land, Crops</t>
   </si>
 </sst>
 </file>
@@ -1737,8 +1767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F8064A-38A3-204E-961F-DB16C98FA406}">
   <dimension ref="A1:Q91"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView topLeftCell="E61" workbookViewId="0">
+      <selection activeCell="N82" sqref="N82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6403,10 +6433,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4800B10-C144-324B-AB72-3BE199CF63FA}">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6416,6 +6446,8 @@
     <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -7035,7 +7067,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="15"/>
       <c r="B33" t="s">
         <v>40</v>
@@ -7053,7 +7085,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
         <v>423</v>
       </c>
@@ -7067,7 +7099,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
         <v>408</v>
       </c>
@@ -7087,7 +7119,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
       <c r="B38" t="s">
         <v>22</v>
@@ -7111,7 +7143,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" t="s">
         <v>23</v>
@@ -7135,7 +7167,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" t="s">
         <v>24</v>
@@ -7159,7 +7191,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" t="s">
         <v>25</v>
@@ -7177,7 +7209,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" t="s">
         <v>26</v>
@@ -7201,7 +7233,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" t="s">
         <v>27</v>
@@ -7219,7 +7251,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" t="s">
         <v>28</v>
@@ -7231,16 +7263,34 @@
         <v>414</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="18"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="19"/>
       <c r="B46" s="6" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C46" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="K46" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="M46" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="O46" s="6" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
         <v>408</v>
       </c>
@@ -7253,8 +7303,17 @@
       <c r="D47" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J47" t="s">
+        <v>29</v>
+      </c>
+      <c r="K47" t="s">
+        <v>29</v>
+      </c>
+      <c r="L47" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="17"/>
       <c r="B48" t="s">
         <v>30</v>
@@ -7274,8 +7333,32 @@
       <c r="G48" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H48" t="s">
+        <v>430</v>
+      </c>
+      <c r="J48" t="s">
+        <v>426</v>
+      </c>
+      <c r="K48" t="s">
+        <v>29</v>
+      </c>
+      <c r="L48" t="s">
+        <v>350</v>
+      </c>
+      <c r="M48" t="s">
+        <v>239</v>
+      </c>
+      <c r="N48" t="s">
+        <v>264</v>
+      </c>
+      <c r="O48" t="s">
+        <v>428</v>
+      </c>
+      <c r="P48" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="17"/>
       <c r="B49" t="s">
         <v>34</v>
@@ -7286,8 +7369,17 @@
       <c r="D49" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J49" t="s">
+        <v>34</v>
+      </c>
+      <c r="K49" t="s">
+        <v>34</v>
+      </c>
+      <c r="L49" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="17"/>
       <c r="B50" t="s">
         <v>35</v>
@@ -7306,6 +7398,30 @@
       </c>
       <c r="G50" t="s">
         <v>117</v>
+      </c>
+      <c r="H50" t="s">
+        <v>431</v>
+      </c>
+      <c r="J50" t="s">
+        <v>427</v>
+      </c>
+      <c r="K50" t="s">
+        <v>34</v>
+      </c>
+      <c r="L50" t="s">
+        <v>351</v>
+      </c>
+      <c r="M50" t="s">
+        <v>239</v>
+      </c>
+      <c r="N50" t="s">
+        <v>264</v>
+      </c>
+      <c r="O50" t="s">
+        <v>429</v>
+      </c>
+      <c r="P50" t="s">
+        <v>433</v>
       </c>
     </row>
   </sheetData>

</xml_diff>